<commit_message>
[DLG] Added ADC signals to blf_converter script and corresponding signals to CANalyzer config
</commit_message>
<xml_diff>
--- a/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
+++ b/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandboxes\Sewela.com\smart-vibrator\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buderm\repositories\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E01C023-10BF-441D-8E53-7F474FB244F1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB88B1E-137E-48F1-9D45-9681610EB60A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3420" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
+    <workbookView xWindow="28680" yWindow="-4590" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$80</definedName>
+    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
   <si>
     <t>F</t>
   </si>
@@ -217,10 +219,22 @@
     <t>Padding Byte</t>
   </si>
   <si>
-    <t>/8</t>
-  </si>
-  <si>
     <t>Variable name</t>
+  </si>
+  <si>
+    <t>adc_raw_level_f32</t>
+  </si>
+  <si>
+    <t>adc_filtered_level_f32</t>
+  </si>
+  <si>
+    <t>adc_raw_data_u16</t>
+  </si>
+  <si>
+    <t>adc_previous_raw_data_u16</t>
+  </si>
+  <si>
+    <t>adc_voltage_u16</t>
   </si>
 </sst>
 </file>
@@ -252,21 +266,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -298,11 +303,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -310,29 +335,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -346,17 +364,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -670,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A8A1A0-79E1-4920-A494-B8E76457F73A}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,15 +809,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="17"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>56</v>
+      <c r="E1" s="15" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
@@ -721,7 +843,7 @@
         <v>32</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D58" si="0">IF(C3="","",C3/8)</f>
+        <f t="shared" ref="D3:D65" si="0">IF(C3="","",C3/8)</f>
         <v>4</v>
       </c>
       <c r="E3" t="s">
@@ -909,372 +1031,381 @@
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7">
-        <v>32</v>
-      </c>
-      <c r="D16" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="B16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="11">
+        <v>32</v>
+      </c>
+      <c r="D16" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11">
+        <v>32</v>
+      </c>
+      <c r="D17" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="11">
+        <v>32</v>
+      </c>
+      <c r="D18" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="9">
-        <f>COUNT(C2:C16)</f>
-        <v>15</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="1" t="str">
+      <c r="C19" s="6">
+        <f>COUNT(C2:C18)</f>
+        <v>17</v>
+      </c>
+      <c r="D19" s="7">
+        <f>SUM(D2:D18)</f>
+        <v>68</v>
+      </c>
+      <c r="E19" s="8">
+        <f>MOD(D19,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1">
-        <v>32</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E19" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="18">
+        <v>32</v>
+      </c>
+      <c r="D21" s="18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E21" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="7">
-        <v>32</v>
-      </c>
-      <c r="D20" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E20" s="5" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
+        <v>32</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="10" t="s">
+    <row r="23" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="9">
-        <f>COUNT(C19:C20)</f>
+      <c r="C23" s="6">
+        <f>COUNT(C21:C22)</f>
         <v>2</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="14">
+      <c r="D23" s="7">
+        <f>SUM(D21:D22)</f>
+        <v>8</v>
+      </c>
+      <c r="E23" s="8">
+        <f>MOD(D23,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="18">
         <v>16</v>
       </c>
-      <c r="D23" s="14">
-        <f t="shared" ref="D23:D32" si="1">IF(C23="","",C23/8)</f>
+      <c r="D25" s="18">
+        <f t="shared" ref="D25:D37" si="1">IF(C25="","",C25/8)</f>
         <v>2</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E25" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="9">
-        <f>COUNT(C23)</f>
-        <v>1</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="13"/>
-    </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="14">
+      <c r="B26" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="11">
         <v>16</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="11">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>27</v>
+      <c r="E26" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="1">
+      <c r="B27" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="11">
         <v>16</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="11">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E27" t="s">
-        <v>28</v>
+      <c r="E27" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="1">
+      <c r="B28" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11">
         <v>16</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="11">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+      <c r="E28" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="6">
+        <f>COUNT(C25:C28)</f>
+        <v>4</v>
+      </c>
+      <c r="D29" s="7">
+        <f>SUM(D25:D28)</f>
+        <v>8</v>
+      </c>
+      <c r="E29" s="8">
+        <f>MOD(D29,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C31" s="18">
         <v>16</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D31" s="18">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+      <c r="E31" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C32" s="1">
         <v>16</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D32" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C33" s="1">
         <v>16</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D33" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="7" t="s">
+      <c r="E33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C34" s="1">
         <v>16</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D34" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="1">
+        <v>16</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="1">
+        <v>16</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="5">
+        <v>16</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="10" t="s">
+    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="9">
-        <f>COUNT(C26:C32)</f>
+      <c r="C38" s="6">
+        <f>COUNT(C31:C37)</f>
         <v>7</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="3"/>
-      <c r="C35" s="4">
-        <f>SUM(C2:C16,C19:C20,C23:C32)</f>
-        <v>673</v>
-      </c>
-      <c r="D35" s="4">
-        <f>SUM(D2:D16,D19:D20,D23:D32)</f>
-        <v>84</v>
-      </c>
-      <c r="E35" s="3">
-        <f>MOD(D35,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1">
-        <v>8</v>
-      </c>
-      <c r="D37" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E37" s="12" t="s">
+      <c r="D38" s="6">
+        <f>SUM(D31:D37)</f>
+        <v>14</v>
+      </c>
+      <c r="E38" s="8">
+        <f>MOD(D38,4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16">
+        <v>0</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="13"/>
+    </row>
+    <row r="42" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="7">
+        <f>D38+D40</f>
+        <v>14</v>
+      </c>
+      <c r="E42" s="8">
+        <f>MOD(D42,4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="11"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="18">
+        <v>8</v>
+      </c>
+      <c r="D44" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E44" s="20" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1">
-        <v>8</v>
-      </c>
-      <c r="D38" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="1">
-        <v>8</v>
-      </c>
-      <c r="D39" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1">
-        <v>8</v>
-      </c>
-      <c r="D40" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="1">
-        <v>8</v>
-      </c>
-      <c r="D41" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1">
-        <v>8</v>
-      </c>
-      <c r="D42" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="1">
-        <v>8</v>
-      </c>
-      <c r="D43" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="1">
-        <v>8</v>
-      </c>
-      <c r="D44" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
@@ -1288,8 +1419,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E45" s="12" t="s">
-        <v>52</v>
+      <c r="E45" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
@@ -1303,8 +1434,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E46" s="12" t="s">
-        <v>53</v>
+      <c r="E46" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
@@ -1318,8 +1449,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E47" s="12" t="s">
-        <v>2</v>
+      <c r="E47" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
@@ -1333,8 +1464,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E48" s="12" t="s">
-        <v>3</v>
+      <c r="E48" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -1348,8 +1479,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E49" s="12" t="s">
-        <v>4</v>
+      <c r="E49" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
@@ -1363,8 +1494,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E50" s="12" t="s">
-        <v>5</v>
+      <c r="E50" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -1378,8 +1509,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E51" s="12" t="s">
-        <v>7</v>
+      <c r="E51" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
@@ -1393,8 +1524,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E52" s="12" t="s">
-        <v>8</v>
+      <c r="E52" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
@@ -1408,8 +1539,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E53" s="12" t="s">
-        <v>9</v>
+      <c r="E53" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
@@ -1423,8 +1554,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E54" s="12" t="s">
-        <v>10</v>
+      <c r="E54" s="9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -1438,8 +1569,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E55" s="12" t="s">
-        <v>11</v>
+      <c r="E55" s="9" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -1453,38 +1584,38 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E56" s="12" t="s">
-        <v>12</v>
+      <c r="E56" s="9" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="14">
-        <v>8</v>
-      </c>
-      <c r="D57" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>40</v>
+      <c r="B57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1">
+        <v>8</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="14">
-        <v>8</v>
-      </c>
-      <c r="D58" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>13</v>
+      <c r="B58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1">
+        <v>8</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -1495,114 +1626,201 @@
         <v>8</v>
       </c>
       <c r="D59" s="1">
-        <f>IF(C59="","",C59/8)</f>
-        <v>1</v>
-      </c>
-      <c r="E59" s="12" t="s">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1">
+        <v>8</v>
+      </c>
+      <c r="D60" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1">
+        <v>8</v>
+      </c>
+      <c r="D61" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1">
+        <v>8</v>
+      </c>
+      <c r="D62" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1">
+        <v>8</v>
+      </c>
+      <c r="D63" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="11">
+        <v>8</v>
+      </c>
+      <c r="D64" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="11">
+        <v>8</v>
+      </c>
+      <c r="D65" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="1">
+        <v>8</v>
+      </c>
+      <c r="D66" s="1">
+        <f>IF(C66="","",C66/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E66" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="10" t="s">
+    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="9">
-        <f>COUNT(C37:C59)</f>
+      <c r="C67" s="6">
+        <f>COUNT(C44:C66)</f>
         <v>23</v>
       </c>
-      <c r="D60" s="10"/>
-      <c r="E60" s="11"/>
-    </row>
-    <row r="61" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="14"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="13"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="14">
-        <v>8</v>
-      </c>
-      <c r="D62" s="14">
-        <v>1</v>
-      </c>
-      <c r="E62" s="16" t="s">
+      <c r="D67" s="8">
+        <f>SUM(D44:D66)</f>
+        <v>23</v>
+      </c>
+      <c r="E67" s="8">
+        <f>MOD(D67,4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="11"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="10"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16">
+        <v>3</v>
+      </c>
+      <c r="E69" s="17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C63" s="9">
-        <f>COUNT(C62)</f>
-        <v>1</v>
-      </c>
-      <c r="D63" s="10"/>
-      <c r="E63" s="11"/>
-    </row>
-    <row r="64" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="10"/>
-      <c r="C65" s="10">
-        <f>SUM(C37:C62)</f>
-        <v>215</v>
-      </c>
-      <c r="D65" s="10">
-        <f>SUM(D37:D62)</f>
-        <v>24</v>
-      </c>
-      <c r="E65" s="10">
-        <f>MOD(D65,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="10"/>
-      <c r="C67" s="9">
-        <f>SUM(C2:C16,C19:C20,C23,C26:C32,C37:C59,C62)</f>
-        <v>864</v>
-      </c>
-      <c r="D67" s="9">
-        <f>SUM(D2:D16,D19:D20,D23,D26:D32,D37:D59,D62)</f>
-        <v>108</v>
-      </c>
-      <c r="E67" s="10">
-        <f>MOD(D67,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="13"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D68" s="4">
-        <f>C67/8</f>
-        <v>108</v>
-      </c>
-      <c r="E68" s="3"/>
-    </row>
-    <row r="69" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="13"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="13"/>
+    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="7">
+        <f>D67+D69</f>
+        <v>26</v>
+      </c>
+      <c r="E71" s="8">
+        <f>MOD(D71,4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7">
+        <f>SUM(D19,D23,D29,D42,D71)</f>
+        <v>124</v>
+      </c>
+      <c r="E73" s="7">
+        <f>MOD(D73,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="10"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="10"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="10"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="10"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B40:E40">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$D$40&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69:E69">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$D$69&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[DLG, SIM] Added SENSE TS data to simulation environment
</commit_message>
<xml_diff>
--- a/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
+++ b/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buderm\repositories\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB88B1E-137E-48F1-9D45-9681610EB60A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D55CB40-4F33-4B55-A95B-F304E2E2D11A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-4590" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$85</definedName>
+    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$89</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
   <si>
     <t>F</t>
   </si>
@@ -235,6 +235,18 @@
   </si>
   <si>
     <t>adc_voltage_u16</t>
+  </si>
+  <si>
+    <t>sense_ts_alpha_filtered_adc_level_f32</t>
+  </si>
+  <si>
+    <t>sense_ts_alpha_beta_filtered_adc_level_f32</t>
+  </si>
+  <si>
+    <t>sense_ts_touch_confidence_f32</t>
+  </si>
+  <si>
+    <t>sense_ts_touch_confidence_max_f32</t>
   </si>
 </sst>
 </file>
@@ -387,77 +399,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -792,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A8A1A0-79E1-4920-A494-B8E76457F73A}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +746,7 @@
     <col min="2" max="2" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -843,7 +785,7 @@
         <v>32</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D65" si="0">IF(C3="","",C3/8)</f>
+        <f t="shared" ref="D3:D69" si="0">IF(C3="","",C3/8)</f>
         <v>4</v>
       </c>
       <c r="E3" t="s">
@@ -1075,70 +1017,77 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>32</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" ref="D19:D22" si="1">IF(C19="","",C19/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>32</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="11">
+        <v>32</v>
+      </c>
+      <c r="D21" s="11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="11">
+        <v>32</v>
+      </c>
+      <c r="D22" s="11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="6">
-        <f>COUNT(C2:C18)</f>
-        <v>17</v>
-      </c>
-      <c r="D19" s="7">
-        <f>SUM(D2:D18)</f>
-        <v>68</v>
-      </c>
-      <c r="E19" s="8">
-        <f>MOD(D19,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="18">
-        <v>32</v>
-      </c>
-      <c r="D21" s="18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="5">
-        <v>32</v>
-      </c>
-      <c r="D22" s="5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="8" t="s">
-        <v>43</v>
-      </c>
       <c r="C23" s="6">
-        <f>COUNT(C21:C22)</f>
-        <v>2</v>
+        <f>COUNT(C2:C22)</f>
+        <v>21</v>
       </c>
       <c r="D23" s="7">
-        <f>SUM(D21:D22)</f>
-        <v>8</v>
+        <f>SUM(D2:D22)</f>
+        <v>84</v>
       </c>
       <c r="E23" s="8">
         <f>MOD(D23,4)</f>
@@ -1146,164 +1095,157 @@
       </c>
     </row>
     <row r="24" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="2"/>
+      <c r="D24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="18">
+        <v>32</v>
+      </c>
+      <c r="D25" s="18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5">
+        <v>32</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="6">
+        <f>COUNT(C25:C26)</f>
+        <v>2</v>
+      </c>
+      <c r="D27" s="7">
+        <f>SUM(D25:D26)</f>
+        <v>8</v>
+      </c>
+      <c r="E27" s="8">
+        <f>MOD(D27,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="18">
         <v>16</v>
       </c>
-      <c r="D25" s="18">
-        <f t="shared" ref="D25:D37" si="1">IF(C25="","",C25/8)</f>
+      <c r="D29" s="18">
+        <f t="shared" ref="D29:D41" si="2">IF(C29="","",C29/8)</f>
         <v>2</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E29" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="11">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="11">
         <v>16</v>
       </c>
-      <c r="D26" s="11">
-        <f t="shared" si="1"/>
+      <c r="D30" s="11">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="11">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="11">
         <v>16</v>
       </c>
-      <c r="D27" s="11">
-        <f t="shared" si="1"/>
+      <c r="D31" s="11">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E31" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="11">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="11">
         <v>16</v>
       </c>
-      <c r="D28" s="11">
-        <f t="shared" si="1"/>
+      <c r="D32" s="11">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="8" t="s">
+    <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="6">
-        <f>COUNT(C25:C28)</f>
-        <v>4</v>
-      </c>
-      <c r="D29" s="7">
-        <f>SUM(D25:D28)</f>
-        <v>8</v>
-      </c>
-      <c r="E29" s="8">
-        <f>MOD(D29,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="18" t="s">
+      <c r="C33" s="6">
+        <f>COUNT(C29:C32)</f>
+        <v>4</v>
+      </c>
+      <c r="D33" s="7">
+        <f>SUM(D29:D32)</f>
+        <v>8</v>
+      </c>
+      <c r="E33" s="8">
+        <f>MOD(D33,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C35" s="18">
         <v>16</v>
       </c>
-      <c r="D31" s="18">
-        <f t="shared" si="1"/>
+      <c r="D35" s="18">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E35" s="19" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="1">
-        <v>16</v>
-      </c>
-      <c r="D32" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="1">
-        <v>16</v>
-      </c>
-      <c r="D33" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="1">
-        <v>16</v>
-      </c>
-      <c r="D34" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="1">
-        <v>16</v>
-      </c>
-      <c r="D35" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E35" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -1314,72 +1256,98 @@
         <v>16</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="1">
         <v>16</v>
       </c>
-      <c r="D37" s="5">
-        <f t="shared" si="1"/>
+      <c r="D37" s="1">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="1">
+        <v>16</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="1">
+        <v>16</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="5">
+        <v>16</v>
+      </c>
+      <c r="D41" s="5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="8" t="s">
+    <row r="42" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="6">
-        <f>COUNT(C31:C37)</f>
+      <c r="C42" s="6">
+        <f>COUNT(C35:C41)</f>
         <v>7</v>
       </c>
-      <c r="D38" s="6">
-        <f>SUM(D31:D37)</f>
-        <v>14</v>
-      </c>
-      <c r="E38" s="8">
-        <f>MOD(D38,4)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16">
-        <v>0</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="13"/>
-    </row>
-    <row r="42" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="7">
-        <f>D38+D40</f>
+      <c r="D42" s="6">
+        <f>SUM(D35:D41)</f>
         <v>14</v>
       </c>
       <c r="E42" s="8">
@@ -1388,84 +1356,58 @@
       </c>
     </row>
     <row r="43" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="10"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="3"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="18">
-        <v>8</v>
-      </c>
-      <c r="D44" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E44" s="20" t="s">
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16">
+        <v>0</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="13"/>
+    </row>
+    <row r="46" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="7">
+        <f>D42+D44</f>
+        <v>14</v>
+      </c>
+      <c r="E46" s="8">
+        <f>MOD(D46,4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="11"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="18">
+        <v>8</v>
+      </c>
+      <c r="D48" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E48" s="20" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="1">
-        <v>8</v>
-      </c>
-      <c r="D45" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="1">
-        <v>8</v>
-      </c>
-      <c r="D46" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="1">
-        <v>8</v>
-      </c>
-      <c r="D47" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1">
-        <v>8</v>
-      </c>
-      <c r="D48" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -1480,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
@@ -1495,7 +1437,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -1510,7 +1452,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
@@ -1525,7 +1467,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
@@ -1540,7 +1482,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
@@ -1555,7 +1497,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -1570,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -1585,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -1600,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -1615,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -1630,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
@@ -1645,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
@@ -1660,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
@@ -1675,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
@@ -1690,37 +1632,37 @@
         <v>1</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="11">
-        <v>8</v>
-      </c>
-      <c r="D64" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E64" s="13" t="s">
-        <v>40</v>
+      <c r="B64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="1">
+        <v>8</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="11">
-        <v>8</v>
-      </c>
-      <c r="D65" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E65" s="13" t="s">
-        <v>13</v>
+      <c r="B65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="1">
+        <v>8</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1731,94 +1673,154 @@
         <v>8</v>
       </c>
       <c r="D66" s="1">
-        <f>IF(C66="","",C66/8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E66" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="1">
+        <v>8</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="11">
+        <v>8</v>
+      </c>
+      <c r="D68" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="11">
+        <v>8</v>
+      </c>
+      <c r="D69" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="1">
+        <v>8</v>
+      </c>
+      <c r="D70" s="1">
+        <f>IF(C70="","",C70/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E70" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="8" t="s">
+    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C67" s="6">
-        <f>COUNT(C44:C66)</f>
+      <c r="C71" s="6">
+        <f>COUNT(C48:C70)</f>
         <v>23</v>
       </c>
-      <c r="D67" s="8">
-        <f>SUM(D44:D66)</f>
+      <c r="D71" s="8">
+        <f>SUM(D48:D70)</f>
         <v>23</v>
-      </c>
-      <c r="E67" s="8">
-        <f>MOD(D67,4)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="11"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="10"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="16"/>
-      <c r="C69" s="16"/>
-      <c r="D69" s="16">
-        <v>3</v>
-      </c>
-      <c r="E69" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="7">
-        <f>D67+D69</f>
-        <v>26</v>
       </c>
       <c r="E71" s="8">
         <f>MOD(D71,4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="11"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="10"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16">
+        <v>3</v>
+      </c>
+      <c r="E73" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="7">
+        <f>D71+D73</f>
+        <v>26</v>
+      </c>
+      <c r="E75" s="8">
+        <f>MOD(D75,4)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7">
-        <f>SUM(D19,D23,D29,D42,D71)</f>
-        <v>124</v>
-      </c>
-      <c r="E73" s="7">
-        <f>MOD(D73,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="10"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="10"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="10"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="10"/>
+    <row r="76" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7">
+        <f>SUM(D23,D27,D33,D46,D75)</f>
+        <v>140</v>
+      </c>
+      <c r="E77" s="7">
+        <f>MOD(D77,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="10"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="10"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="10"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B40:E40">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$D$40&gt;0</formula>
+  <conditionalFormatting sqref="B44:E44">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$D$44&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B69:E69">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$D$69&gt;0</formula>
+  <conditionalFormatting sqref="B73:E73">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$D$73&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[DD, DLG] Added database dd_ina_219_data_s into logging domain
</commit_message>
<xml_diff>
--- a/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
+++ b/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buderm\repositories\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandboxes\Sewela.com\smart-vibrator\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D55CB40-4F33-4B55-A95B-F304E2E2D11A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3C0734-1E9D-428D-8665-FEE4EE61461B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4590" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
+    <workbookView xWindow="28680" yWindow="-3195" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$89</definedName>
+    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
   <si>
     <t>F</t>
   </si>
@@ -247,6 +247,39 @@
   </si>
   <si>
     <t>sense_ts_touch_confidence_max_f32</t>
+  </si>
+  <si>
+    <t>dd_ina_219_shunt_voltage_mV_f32</t>
+  </si>
+  <si>
+    <t>dd_ina_219_bus_voltage_V_f32</t>
+  </si>
+  <si>
+    <t>dd_ina_219_power_mW_f32</t>
+  </si>
+  <si>
+    <t>dd_ina_219_current_mA_f32</t>
+  </si>
+  <si>
+    <t>dd_ina_219_shunt_voltage_raw_u16</t>
+  </si>
+  <si>
+    <t>dd_ina_219_power_raw_u16</t>
+  </si>
+  <si>
+    <t>dd_ina_219_current_raw_u16</t>
+  </si>
+  <si>
+    <t>dd_ina_219_bus_voltage_raw_u16</t>
+  </si>
+  <si>
+    <t>dd_ina_219_shunt_voltage_range_u8</t>
+  </si>
+  <si>
+    <t>dd_ina_219_bus_voltage_range_u8</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -376,12 +409,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -394,6 +421,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,16 +767,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A8A1A0-79E1-4920-A494-B8E76457F73A}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
@@ -751,14 +784,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="14"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="20" t="s">
         <v>55</v>
       </c>
     </row>
@@ -785,7 +820,7 @@
         <v>32</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D69" si="0">IF(C3="","",C3/8)</f>
+        <f t="shared" ref="D3:D77" si="0">IF(C3="","",C3/8)</f>
         <v>4</v>
       </c>
       <c r="E3" t="s">
@@ -1025,7 +1060,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" ref="D19:D22" si="1">IF(C19="","",C19/8)</f>
+        <f t="shared" ref="D19:D23" si="1">IF(C19="","",C19/8)</f>
         <v>4</v>
       </c>
       <c r="E19" s="10" t="s">
@@ -1077,70 +1112,76 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="11">
+        <v>32</v>
+      </c>
+      <c r="D23" s="11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>32</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" ref="D24:D25" si="2">IF(C24="","",C24/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>32</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="11">
+        <v>32</v>
+      </c>
+      <c r="D26" s="11">
+        <v>4</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="6">
-        <f>COUNT(C2:C22)</f>
-        <v>21</v>
-      </c>
-      <c r="D23" s="7">
-        <f>SUM(D2:D22)</f>
-        <v>84</v>
-      </c>
-      <c r="E23" s="8">
-        <f>MOD(D23,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="18">
-        <v>32</v>
-      </c>
-      <c r="D25" s="18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="5">
-        <v>32</v>
-      </c>
-      <c r="D26" s="5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="C27" s="7">
+        <f>COUNT(C2:C26)</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="6">
-        <f>COUNT(C25:C26)</f>
-        <v>2</v>
-      </c>
       <c r="D27" s="7">
-        <f>SUM(D25:D26)</f>
-        <v>8</v>
+        <f>SUM(D2:D26)</f>
+        <v>100</v>
       </c>
       <c r="E27" s="8">
         <f>MOD(D27,4)</f>
@@ -1148,386 +1189,379 @@
       </c>
     </row>
     <row r="28" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="2"/>
+      <c r="D28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="18">
+      <c r="B29" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="16">
+        <v>32</v>
+      </c>
+      <c r="D29" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5">
+        <v>32</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="7">
+        <f>COUNT(C29:C30)</f>
+        <v>2</v>
+      </c>
+      <c r="D31" s="7">
+        <f>SUM(D29:D30)</f>
+        <v>8</v>
+      </c>
+      <c r="E31" s="8">
+        <f>MOD(D31,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="16">
         <v>16</v>
       </c>
-      <c r="D29" s="18">
-        <f t="shared" ref="D29:D41" si="2">IF(C29="","",C29/8)</f>
+      <c r="D33" s="16">
+        <f t="shared" ref="D33:D49" si="3">IF(C33="","",C33/8)</f>
         <v>2</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E33" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="11">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="11">
         <v>16</v>
       </c>
-      <c r="D30" s="11">
-        <f t="shared" si="2"/>
+      <c r="D34" s="11">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="11">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="11">
         <v>16</v>
       </c>
-      <c r="D31" s="11">
-        <f t="shared" si="2"/>
+      <c r="D35" s="11">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E35" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="11">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="11">
         <v>16</v>
       </c>
-      <c r="D32" s="11">
-        <f t="shared" si="2"/>
+      <c r="D36" s="11">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E36" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="8" t="s">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="11">
+        <v>16</v>
+      </c>
+      <c r="D37" s="11">
+        <f t="shared" ref="D37:D40" si="4">IF(C37="","",C37/8)</f>
+        <v>2</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="11">
+        <v>16</v>
+      </c>
+      <c r="D38" s="11">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="11">
+        <v>16</v>
+      </c>
+      <c r="D39" s="11">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="11">
+        <v>16</v>
+      </c>
+      <c r="D40" s="11">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="6">
-        <f>COUNT(C29:C32)</f>
-        <v>4</v>
-      </c>
-      <c r="D33" s="7">
-        <f>SUM(D29:D32)</f>
-        <v>8</v>
-      </c>
-      <c r="E33" s="8">
-        <f>MOD(D33,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="18" t="s">
+      <c r="C41" s="7">
+        <f>COUNT(C33:C40)</f>
+        <v>8</v>
+      </c>
+      <c r="D41" s="7">
+        <f>SUM(D33:D40)</f>
+        <v>16</v>
+      </c>
+      <c r="E41" s="8">
+        <f>MOD(D41,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C43" s="16">
         <v>16</v>
       </c>
-      <c r="D35" s="18">
-        <f t="shared" si="2"/>
+      <c r="D43" s="16">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E43" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C44" s="1">
         <v>16</v>
       </c>
-      <c r="D36" s="1">
-        <f t="shared" si="2"/>
+      <c r="D44" s="1">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C45" s="1">
         <v>16</v>
       </c>
-      <c r="D37" s="1">
-        <f t="shared" si="2"/>
+      <c r="D45" s="1">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C46" s="1">
         <v>16</v>
       </c>
-      <c r="D38" s="1">
-        <f t="shared" si="2"/>
+      <c r="D46" s="1">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E46" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C47" s="1">
         <v>16</v>
       </c>
-      <c r="D39" s="1">
-        <f t="shared" si="2"/>
+      <c r="D47" s="1">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E47" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C48" s="1">
         <v>16</v>
       </c>
-      <c r="D40" s="1">
-        <f t="shared" si="2"/>
+      <c r="D48" s="1">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="5" t="s">
+      <c r="E48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C49" s="5">
         <v>16</v>
       </c>
-      <c r="D41" s="5">
-        <f t="shared" si="2"/>
+      <c r="D49" s="5">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="8" t="s">
+    <row r="50" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="6">
-        <f>COUNT(C35:C41)</f>
+      <c r="C50" s="7">
+        <f>COUNT(C43:C49)</f>
         <v>7</v>
       </c>
-      <c r="D42" s="6">
-        <f>SUM(D35:D41)</f>
+      <c r="D50" s="6">
+        <f>SUM(D43:D49)</f>
         <v>14</v>
       </c>
-      <c r="E42" s="8">
-        <f>MOD(D42,4)</f>
+      <c r="E50" s="8">
+        <f>MOD(D50,4)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="5"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16">
-        <v>0</v>
-      </c>
-      <c r="E44" s="17" t="s">
+    <row r="51" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14">
+        <v>0</v>
+      </c>
+      <c r="E52" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="13"/>
-    </row>
-    <row r="46" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="7">
-        <f>D42+D44</f>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="13"/>
+    </row>
+    <row r="54" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="7">
+        <f>D50+D52</f>
         <v>14</v>
       </c>
-      <c r="E46" s="8">
-        <f>MOD(D46,4)</f>
+      <c r="E54" s="8">
+        <f>MOD(D54,4)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="11"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="10"/>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="18">
-        <v>8</v>
-      </c>
-      <c r="D48" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E48" s="20" t="s">
+    <row r="55" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="11"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="10"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="16">
+        <v>8</v>
+      </c>
+      <c r="D56" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E56" s="18" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="1">
-        <v>8</v>
-      </c>
-      <c r="D49" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1">
-        <v>8</v>
-      </c>
-      <c r="D50" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="1">
-        <v>8</v>
-      </c>
-      <c r="D51" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="1">
-        <v>8</v>
-      </c>
-      <c r="D52" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="1">
-        <v>8</v>
-      </c>
-      <c r="D53" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1">
-        <v>8</v>
-      </c>
-      <c r="D54" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="1">
-        <v>8</v>
-      </c>
-      <c r="D55" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1">
-        <v>8</v>
-      </c>
-      <c r="D56" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -1542,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -1557,7 +1591,7 @@
         <v>1</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -1572,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
@@ -1587,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
@@ -1602,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
@@ -1617,7 +1651,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
@@ -1632,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
@@ -1647,180 +1681,330 @@
         <v>1</v>
       </c>
       <c r="E64" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="1">
+        <v>8</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="1">
+        <v>8</v>
+      </c>
+      <c r="D66" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="1">
+        <v>8</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="1">
+        <v>8</v>
+      </c>
+      <c r="D68" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="1">
+        <v>8</v>
+      </c>
+      <c r="D69" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="1">
+        <v>8</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="1">
+        <v>8</v>
+      </c>
+      <c r="D71" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="1">
+        <v>8</v>
+      </c>
+      <c r="D72" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E72" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="1">
-        <v>8</v>
-      </c>
-      <c r="D65" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E65" s="9" t="s">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="1">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E73" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="1">
-        <v>8</v>
-      </c>
-      <c r="D66" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E66" s="9" t="s">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="1">
+        <v>8</v>
+      </c>
+      <c r="D74" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E74" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="1">
-        <v>8</v>
-      </c>
-      <c r="D67" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E67" s="9" t="s">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="1">
+        <v>8</v>
+      </c>
+      <c r="D75" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E75" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="11">
-        <v>8</v>
-      </c>
-      <c r="D68" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E68" s="13" t="s">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="11">
+        <v>8</v>
+      </c>
+      <c r="D76" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E76" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C69" s="11">
-        <v>8</v>
-      </c>
-      <c r="D69" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E69" s="13" t="s">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="11">
+        <v>8</v>
+      </c>
+      <c r="D77" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E77" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" s="1">
-        <v>8</v>
-      </c>
-      <c r="D70" s="1">
-        <f>IF(C70="","",C70/8)</f>
-        <v>1</v>
-      </c>
-      <c r="E70" s="9" t="s">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="1">
+        <v>8</v>
+      </c>
+      <c r="D78" s="1">
+        <f t="shared" ref="D78:D79" si="5">IF(C78="","",C78/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E78" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="1">
+        <v>8</v>
+      </c>
+      <c r="D79" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" s="1">
+        <v>8</v>
+      </c>
+      <c r="D80" s="1">
+        <f>IF(C80="","",C80/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E80" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="8" t="s">
+    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C71" s="6">
-        <f>COUNT(C48:C70)</f>
-        <v>23</v>
-      </c>
-      <c r="D71" s="8">
-        <f>SUM(D48:D70)</f>
-        <v>23</v>
-      </c>
-      <c r="E71" s="8">
-        <f>MOD(D71,4)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="11"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="10"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="16"/>
-      <c r="C73" s="16"/>
-      <c r="D73" s="16">
-        <v>3</v>
-      </c>
-      <c r="E73" s="17" t="s">
+      <c r="C81" s="7">
+        <f>COUNT(C56:C80)</f>
+        <v>25</v>
+      </c>
+      <c r="D81" s="7">
+        <f>SUM(D56:D80)</f>
+        <v>25</v>
+      </c>
+      <c r="E81" s="8">
+        <f>MOD(D81,4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="11"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="10"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14">
+        <v>1</v>
+      </c>
+      <c r="E83" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="7">
-        <f>D71+D73</f>
+    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="7">
+        <f>D81+D83</f>
         <v>26</v>
       </c>
-      <c r="E75" s="8">
-        <f>MOD(D75,4)</f>
+      <c r="E85" s="8">
+        <f>MOD(D85,4)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7">
-        <f>SUM(D23,D27,D33,D46,D75)</f>
-        <v>140</v>
-      </c>
-      <c r="E77" s="7">
-        <f>MOD(D77,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="10"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="10"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="10"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="10"/>
+    <row r="86" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7">
+        <f>SUM(D27,D31,D41,D54,D85)</f>
+        <v>164</v>
+      </c>
+      <c r="E87" s="7">
+        <f>MOD(D87,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="10"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="10"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="10"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B44:E44">
+  <conditionalFormatting sqref="B52:E52">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$D$44&gt;0</formula>
+      <formula>$D$52&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B73:E73">
+  <conditionalFormatting sqref="B83:E83">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$D$73&gt;0</formula>
+      <formula>$D$83&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[SIM] Added database dd_mcpwm_data_s to data logging
</commit_message>
<xml_diff>
--- a/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
+++ b/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandboxes\Sewela.com\smart-vibrator\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3C0734-1E9D-428D-8665-FEE4EE61461B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14253C7-D51D-41BE-AE9C-B42261B010CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3195" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
+    <workbookView xWindow="28680" yWindow="-3420" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$99</definedName>
+    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$123</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="100">
   <si>
     <t>F</t>
   </si>
@@ -280,13 +280,85 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_1_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_2_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_3_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_4_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_5_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_6_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_7_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_8_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_9_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_10_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_11_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_12_duty_cycle_f32</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_1_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_2_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_3_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_4_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_5_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_6_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_7_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_8_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_9_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_10_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_11_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_mcpwm_ch_12_mode_u8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +370,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -372,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -428,6 +506,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -767,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A8A1A0-79E1-4920-A494-B8E76457F73A}">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +899,7 @@
         <v>32</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D77" si="0">IF(C3="","",C3/8)</f>
+        <f t="shared" ref="D3:D89" si="0">IF(C3="","",C3/8)</f>
         <v>4</v>
       </c>
       <c r="E3" t="s">
@@ -1171,577 +1250,573 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="7">
-        <f>COUNT(C2:C26)</f>
-        <v>25</v>
-      </c>
-      <c r="D27" s="7">
-        <f>SUM(D2:D26)</f>
-        <v>100</v>
-      </c>
-      <c r="E27" s="8">
-        <f>MOD(D27,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>32</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" ref="D27:D38" si="3">IF(C27="","",C27/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1">
+        <v>32</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="16">
-        <v>32</v>
-      </c>
-      <c r="D29" s="16">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>24</v>
+      <c r="B29" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="11">
+        <v>32</v>
+      </c>
+      <c r="D29" s="11">
+        <v>4</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="5">
-        <v>32</v>
-      </c>
-      <c r="D30" s="5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="7">
-        <f>COUNT(C29:C30)</f>
-        <v>2</v>
-      </c>
-      <c r="D31" s="7">
-        <f>SUM(D29:D30)</f>
-        <v>8</v>
-      </c>
-      <c r="E31" s="8">
-        <f>MOD(D31,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="2"/>
+      <c r="B30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>32</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" ref="D30:D38" si="4">IF(C30="","",C30/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>32</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="11">
+        <v>32</v>
+      </c>
+      <c r="D32" s="11">
+        <v>4</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="16">
-        <v>16</v>
-      </c>
-      <c r="D33" s="16">
-        <f t="shared" ref="D33:D49" si="3">IF(C33="","",C33/8)</f>
-        <v>2</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>26</v>
+      <c r="B33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>32</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" ref="D33:D38" si="5">IF(C33="","",C33/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" s="11">
-        <v>16</v>
-      </c>
-      <c r="D34" s="11">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>58</v>
+      <c r="B34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1">
+        <v>32</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="11">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D35" s="11">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>59</v>
+        <v>4</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="11">
-        <v>16</v>
-      </c>
-      <c r="D36" s="11">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>60</v>
+      <c r="B36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>32</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" ref="D36:D38" si="6">IF(C36="","",C36/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="11">
-        <v>16</v>
-      </c>
-      <c r="D37" s="11">
-        <f t="shared" ref="D37:D40" si="4">IF(C37="","",C37/8)</f>
-        <v>2</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>69</v>
+      <c r="B37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>32</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" s="11">
+        <v>32</v>
+      </c>
+      <c r="D38" s="11">
+        <v>4</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="7">
+        <f>COUNT(C2:C38)</f>
+        <v>37</v>
+      </c>
+      <c r="D39" s="7">
+        <f>SUM(D2:D38)</f>
+        <v>148</v>
+      </c>
+      <c r="E39" s="8">
+        <f>MOD(D39,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="16">
+        <v>32</v>
+      </c>
+      <c r="D41" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="5">
+        <v>32</v>
+      </c>
+      <c r="D42" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="7">
+        <f>COUNT(C41:C42)</f>
+        <v>2</v>
+      </c>
+      <c r="D43" s="7">
+        <f>SUM(D41:D42)</f>
+        <v>8</v>
+      </c>
+      <c r="E43" s="8">
+        <f>MOD(D43,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="16">
         <v>16</v>
       </c>
-      <c r="D38" s="11">
-        <f t="shared" si="4"/>
+      <c r="D45" s="16">
+        <f t="shared" ref="D45:D61" si="7">IF(C45="","",C45/8)</f>
         <v>2</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E45" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="11">
+        <v>16</v>
+      </c>
+      <c r="D46" s="11">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="11">
+        <v>16</v>
+      </c>
+      <c r="D47" s="11">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="11">
+        <v>16</v>
+      </c>
+      <c r="D48" s="11">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="11">
+        <v>16</v>
+      </c>
+      <c r="D49" s="11">
+        <f t="shared" ref="D49:D52" si="8">IF(C49="","",C49/8)</f>
+        <v>2</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="11">
+        <v>16</v>
+      </c>
+      <c r="D50" s="11">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E50" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="11">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="11">
         <v>16</v>
       </c>
-      <c r="D39" s="11">
-        <f t="shared" si="4"/>
+      <c r="D51" s="11">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E51" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="11">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="11">
         <v>16</v>
       </c>
-      <c r="D40" s="11">
-        <f t="shared" si="4"/>
+      <c r="D52" s="11">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E52" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="8" t="s">
+    <row r="53" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="7">
-        <f>COUNT(C33:C40)</f>
-        <v>8</v>
-      </c>
-      <c r="D41" s="7">
-        <f>SUM(D33:D40)</f>
+      <c r="C53" s="7">
+        <f>COUNT(C45:C52)</f>
+        <v>8</v>
+      </c>
+      <c r="D53" s="7">
+        <f>SUM(D45:D52)</f>
         <v>16</v>
       </c>
-      <c r="E41" s="8">
-        <f>MOD(D41,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="10"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="16" t="s">
+      <c r="E53" s="8">
+        <f>MOD(D53,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="16">
+      <c r="C55" s="16">
         <v>16</v>
       </c>
-      <c r="D43" s="16">
-        <f t="shared" si="3"/>
+      <c r="D55" s="16">
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E55" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C56" s="1">
         <v>16</v>
       </c>
-      <c r="D44" s="1">
-        <f t="shared" si="3"/>
+      <c r="D56" s="1">
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E56" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="1">
-        <v>16</v>
-      </c>
-      <c r="D45" s="1">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="E45" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="1">
-        <v>16</v>
-      </c>
-      <c r="D46" s="1">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="E46" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="1">
-        <v>16</v>
-      </c>
-      <c r="D47" s="1">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="E47" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="1">
-        <v>16</v>
-      </c>
-      <c r="D48" s="1">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="E48" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" s="5">
-        <v>16</v>
-      </c>
-      <c r="D49" s="5">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="7">
-        <f>COUNT(C43:C49)</f>
-        <v>7</v>
-      </c>
-      <c r="D50" s="6">
-        <f>SUM(D43:D49)</f>
-        <v>14</v>
-      </c>
-      <c r="E50" s="8">
-        <f>MOD(D50,4)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="5"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14">
-        <v>0</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="13"/>
-    </row>
-    <row r="54" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="7">
-        <f>D50+D52</f>
-        <v>14</v>
-      </c>
-      <c r="E54" s="8">
-        <f>MOD(D54,4)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="11"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="10"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="16">
-        <v>8</v>
-      </c>
-      <c r="D56" s="16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E56" s="18" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C57" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>46</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C58" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>47</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C59" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>48</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C60" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>49</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E60" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="1">
-        <v>8</v>
-      </c>
-      <c r="D61" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1">
-        <v>8</v>
-      </c>
-      <c r="D62" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="1">
-        <v>8</v>
-      </c>
-      <c r="D63" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="B61" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="5">
+        <v>16</v>
+      </c>
+      <c r="D61" s="5">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="7">
+        <f>COUNT(C55:C61)</f>
+        <v>7</v>
+      </c>
+      <c r="D62" s="6">
+        <f>SUM(D55:D61)</f>
+        <v>14</v>
+      </c>
+      <c r="E62" s="8">
+        <f>MOD(D62,4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="5"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="3"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="1">
-        <v>8</v>
-      </c>
-      <c r="D64" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>52</v>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14">
+        <v>0</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="1">
-        <v>8</v>
-      </c>
-      <c r="D65" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="1">
-        <v>8</v>
-      </c>
-      <c r="D66" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E66" s="9" t="s">
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="13"/>
+    </row>
+    <row r="66" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="7">
+        <f>D62+D64</f>
+        <v>14</v>
+      </c>
+      <c r="E66" s="8">
+        <f>MOD(D66,4)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="1">
-        <v>8</v>
-      </c>
-      <c r="D67" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>3</v>
-      </c>
+    <row r="67" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="11"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="10"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="1">
-        <v>8</v>
-      </c>
-      <c r="D68" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>4</v>
+      <c r="B68" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="16">
+        <v>8</v>
+      </c>
+      <c r="D68" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
@@ -1756,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
@@ -1771,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
@@ -1786,7 +1861,7 @@
         <v>1</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
@@ -1801,7 +1876,7 @@
         <v>1</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
@@ -1816,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
@@ -1831,7 +1906,7 @@
         <v>1</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
@@ -1846,37 +1921,37 @@
         <v>1</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C76" s="11">
-        <v>8</v>
-      </c>
-      <c r="D76" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E76" s="13" t="s">
-        <v>40</v>
+      <c r="B76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="1">
+        <v>8</v>
+      </c>
+      <c r="D76" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C77" s="11">
-        <v>8</v>
-      </c>
-      <c r="D77" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E77" s="13" t="s">
-        <v>13</v>
+      <c r="B77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1">
+        <v>8</v>
+      </c>
+      <c r="D77" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
@@ -1887,11 +1962,11 @@
         <v>8</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" ref="D78:D79" si="5">IF(C78="","",C78/8)</f>
-        <v>1</v>
-      </c>
-      <c r="E78" s="13" t="s">
-        <v>73</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
@@ -1902,11 +1977,11 @@
         <v>8</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="E79" s="13" t="s">
-        <v>74</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
@@ -1917,94 +1992,455 @@
         <v>8</v>
       </c>
       <c r="D80" s="1">
-        <f>IF(C80="","",C80/8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E80" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="1">
+        <v>8</v>
+      </c>
+      <c r="D81" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="1">
+        <v>8</v>
+      </c>
+      <c r="D82" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="1">
+        <v>8</v>
+      </c>
+      <c r="D83" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="1">
+        <v>8</v>
+      </c>
+      <c r="D84" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="1">
+        <v>8</v>
+      </c>
+      <c r="D85" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1">
+        <v>8</v>
+      </c>
+      <c r="D86" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="1">
+        <v>8</v>
+      </c>
+      <c r="D87" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="11">
+        <v>8</v>
+      </c>
+      <c r="D88" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E88" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="11">
+        <v>8</v>
+      </c>
+      <c r="D89" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E89" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="1">
+        <v>8</v>
+      </c>
+      <c r="D90" s="1">
+        <f t="shared" ref="D90:D93" si="9">IF(C90="","",C90/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E90" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" s="1">
+        <v>8</v>
+      </c>
+      <c r="D91" s="1">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="11">
+        <v>8</v>
+      </c>
+      <c r="D92" s="11">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E92" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="11">
+        <v>8</v>
+      </c>
+      <c r="D93" s="11">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E93" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="1">
+        <v>8</v>
+      </c>
+      <c r="D94" s="1">
+        <f t="shared" ref="D94:D103" si="10">IF(C94="","",C94/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E94" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="1">
+        <v>8</v>
+      </c>
+      <c r="D95" s="1">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E95" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="11">
+        <v>8</v>
+      </c>
+      <c r="D96" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="11">
+        <v>8</v>
+      </c>
+      <c r="D97" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E97" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="1">
+        <v>8</v>
+      </c>
+      <c r="D98" s="1">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E98" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B99" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" s="1">
+        <v>8</v>
+      </c>
+      <c r="D99" s="1">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E99" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B100" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="11">
+        <v>8</v>
+      </c>
+      <c r="D100" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="11">
+        <v>8</v>
+      </c>
+      <c r="D101" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="1">
+        <v>8</v>
+      </c>
+      <c r="D102" s="1">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E102" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" s="1">
+        <v>8</v>
+      </c>
+      <c r="D103" s="1">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E103" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B104" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1">
+        <v>8</v>
+      </c>
+      <c r="D104" s="1">
+        <f>IF(C104="","",C104/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E104" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="8" t="s">
+    <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C81" s="7">
-        <f>COUNT(C56:C80)</f>
-        <v>25</v>
-      </c>
-      <c r="D81" s="7">
-        <f>SUM(D56:D80)</f>
-        <v>25</v>
-      </c>
-      <c r="E81" s="8">
-        <f>MOD(D81,4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="11"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="10"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="14"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14">
-        <v>1</v>
-      </c>
-      <c r="E83" s="15" t="s">
+      <c r="C105" s="7">
+        <f>COUNT(C68:C104)</f>
+        <v>37</v>
+      </c>
+      <c r="D105" s="7">
+        <f>SUM(D68:D104)</f>
+        <v>37</v>
+      </c>
+      <c r="E105" s="8">
+        <f>MOD(D105,4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="11"/>
+      <c r="C106" s="12"/>
+      <c r="D106" s="11"/>
+      <c r="E106" s="10"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="14"/>
+      <c r="C107" s="14"/>
+      <c r="D107" s="14">
+        <v>1</v>
+      </c>
+      <c r="E107" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="7">
-        <f>D81+D83</f>
-        <v>26</v>
-      </c>
-      <c r="E85" s="8">
-        <f>MOD(D85,4)</f>
+    <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="7">
+        <f>D105+D107</f>
+        <v>38</v>
+      </c>
+      <c r="E109" s="8">
+        <f>MOD(D109,4)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
-      <c r="D87" s="7">
-        <f>SUM(D27,D31,D41,D54,D85)</f>
-        <v>164</v>
-      </c>
-      <c r="E87" s="7">
-        <f>MOD(D87,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="10"/>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="10"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="10"/>
-      <c r="B89" s="11"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
-      <c r="E89" s="10"/>
+    <row r="110" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="7">
+        <f>SUM(D39,D43,D53,D66,D109)</f>
+        <v>224</v>
+      </c>
+      <c r="E111" s="7">
+        <f>MOD(D111,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="10"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+      <c r="E112" s="10"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="10"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
+      <c r="E113" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B52:E52">
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B64:E64">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$D$52&gt;0</formula>
+      <formula>$D$64&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B83:E83">
+  <conditionalFormatting sqref="B107:E107">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$D$83&gt;0</formula>
+      <formula>$D$107&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[DD, DLG] Added TMP102 temperature reading into DLG_LOG_DATA structure
</commit_message>
<xml_diff>
--- a/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
+++ b/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandboxes\Sewela.com\smart-vibrator\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buderm\repositories\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14253C7-D51D-41BE-AE9C-B42261B010CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F78996-2C2A-4C98-90DF-AF83D61C62FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3420" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
+    <workbookView xWindow="28680" yWindow="-4590" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$123</definedName>
+    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$125</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="102">
   <si>
     <t>F</t>
   </si>
@@ -352,6 +352,12 @@
   </si>
   <si>
     <t>dd_mcpwm_ch_12_mode_u8</t>
+  </si>
+  <si>
+    <t>dd_tmp_102_temperature_deg_f32</t>
+  </si>
+  <si>
+    <t>dd_tmp_102_temperature_raw_s16</t>
   </si>
 </sst>
 </file>
@@ -846,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A8A1A0-79E1-4920-A494-B8E76457F73A}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,7 +905,7 @@
         <v>32</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D89" si="0">IF(C3="","",C3/8)</f>
+        <f t="shared" ref="D3:D91" si="0">IF(C3="","",C3/8)</f>
         <v>4</v>
       </c>
       <c r="E3" t="s">
@@ -1251,18 +1257,17 @@
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1">
-        <v>32</v>
-      </c>
-      <c r="D27" s="1">
-        <f t="shared" ref="D27:D38" si="3">IF(C27="","",C27/8)</f>
+      <c r="B27" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="11">
+        <v>32</v>
+      </c>
+      <c r="D27" s="11">
         <v>4</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -1273,40 +1278,40 @@
         <v>32</v>
       </c>
       <c r="D28" s="1">
+        <f t="shared" ref="D28:D29" si="3">IF(C28="","",C28/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
+        <v>32</v>
+      </c>
+      <c r="D29" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="11">
-        <v>32</v>
-      </c>
-      <c r="D29" s="11">
-        <v>4</v>
-      </c>
-      <c r="E29" s="21" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="11">
+        <v>32</v>
+      </c>
+      <c r="D30" s="11">
+        <v>4</v>
+      </c>
+      <c r="E30" s="21" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
-        <v>32</v>
-      </c>
-      <c r="D30" s="1">
-        <f t="shared" ref="D30:D38" si="4">IF(C30="","",C30/8)</f>
-        <v>4</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -1317,40 +1322,40 @@
         <v>32</v>
       </c>
       <c r="D31" s="1">
+        <f t="shared" ref="D31:D32" si="4">IF(C31="","",C31/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1">
+        <v>32</v>
+      </c>
+      <c r="D32" s="1">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E32" s="21" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="11">
-        <v>32</v>
-      </c>
-      <c r="D32" s="11">
-        <v>4</v>
-      </c>
-      <c r="E32" s="21" t="s">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="11">
+        <v>32</v>
+      </c>
+      <c r="D33" s="11">
+        <v>4</v>
+      </c>
+      <c r="E33" s="21" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="1">
-        <v>32</v>
-      </c>
-      <c r="D33" s="1">
-        <f t="shared" ref="D33:D38" si="5">IF(C33="","",C33/8)</f>
-        <v>4</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -1361,40 +1366,40 @@
         <v>32</v>
       </c>
       <c r="D34" s="1">
+        <f t="shared" ref="D34:D35" si="5">IF(C34="","",C34/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>32</v>
+      </c>
+      <c r="D35" s="1">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="E34" s="21" t="s">
+      <c r="E35" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="11">
-        <v>32</v>
-      </c>
-      <c r="D35" s="11">
-        <v>4</v>
-      </c>
-      <c r="E35" s="21" t="s">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="11">
+        <v>32</v>
+      </c>
+      <c r="D36" s="11">
+        <v>4</v>
+      </c>
+      <c r="E36" s="21" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="1">
-        <v>32</v>
-      </c>
-      <c r="D36" s="1">
-        <f t="shared" ref="D36:D38" si="6">IF(C36="","",C36/8)</f>
-        <v>4</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -1405,128 +1410,128 @@
         <v>32</v>
       </c>
       <c r="D37" s="1">
+        <f t="shared" ref="D37:D38" si="6">IF(C37="","",C37/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1">
+        <v>32</v>
+      </c>
+      <c r="D38" s="1">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="E37" s="21" t="s">
+      <c r="E38" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="11">
-        <v>32</v>
-      </c>
-      <c r="D38" s="11">
-        <v>4</v>
-      </c>
-      <c r="E38" s="21" t="s">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="11">
+        <v>32</v>
+      </c>
+      <c r="D39" s="11">
+        <v>4</v>
+      </c>
+      <c r="E39" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="6" t="s">
+    <row r="40" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="7">
-        <f>COUNT(C2:C38)</f>
-        <v>37</v>
-      </c>
-      <c r="D39" s="7">
-        <f>SUM(D2:D38)</f>
-        <v>148</v>
-      </c>
-      <c r="E39" s="8">
-        <f>MOD(D39,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D40" s="1" t="str">
+      <c r="C40" s="7">
+        <f>COUNT(C2:C39)</f>
+        <v>38</v>
+      </c>
+      <c r="D40" s="7">
+        <f>SUM(D2:D39)</f>
+        <v>152</v>
+      </c>
+      <c r="E40" s="8">
+        <f>MOD(D40,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="16">
-        <v>32</v>
-      </c>
-      <c r="D41" s="16">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E41" s="17" t="s">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="16">
+        <v>32</v>
+      </c>
+      <c r="D42" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E42" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="5">
-        <v>32</v>
-      </c>
-      <c r="D42" s="5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E42" s="3" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="5">
+        <v>32</v>
+      </c>
+      <c r="D43" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="8" t="s">
+    <row r="44" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="7">
-        <f>COUNT(C41:C42)</f>
+      <c r="C44" s="7">
+        <f>COUNT(C42:C43)</f>
         <v>2</v>
       </c>
-      <c r="D43" s="7">
-        <f>SUM(D41:D42)</f>
-        <v>8</v>
-      </c>
-      <c r="E43" s="8">
-        <f>MOD(D43,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="16">
+      <c r="D44" s="7">
+        <f>SUM(D42:D43)</f>
+        <v>8</v>
+      </c>
+      <c r="E44" s="8">
+        <f>MOD(D44,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="16">
         <v>16</v>
       </c>
-      <c r="D45" s="16">
-        <f t="shared" ref="D45:D61" si="7">IF(C45="","",C45/8)</f>
+      <c r="D46" s="16">
+        <f t="shared" ref="D46:D62" si="7">IF(C46="","",C46/8)</f>
         <v>2</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E46" s="17" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="11">
-        <v>16</v>
-      </c>
-      <c r="D46" s="11">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
@@ -1541,7 +1546,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
@@ -1556,7 +1561,7 @@
         <v>2</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -1567,11 +1572,11 @@
         <v>16</v>
       </c>
       <c r="D49" s="11">
-        <f t="shared" ref="D49:D52" si="8">IF(C49="","",C49/8)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
@@ -1582,11 +1587,11 @@
         <v>16</v>
       </c>
       <c r="D50" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="D50:D53" si="8">IF(C50="","",C50/8)</f>
         <v>2</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -1601,7 +1606,7 @@
         <v>2</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
@@ -1616,60 +1621,60 @@
         <v>2</v>
       </c>
       <c r="E52" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="11">
+        <v>16</v>
+      </c>
+      <c r="D53" s="11">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E53" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="8" t="s">
+    <row r="54" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="7">
-        <f>COUNT(C45:C52)</f>
-        <v>8</v>
-      </c>
-      <c r="D53" s="7">
-        <f>SUM(D45:D52)</f>
+      <c r="C54" s="7">
+        <f>COUNT(C46:C53)</f>
+        <v>8</v>
+      </c>
+      <c r="D54" s="7">
+        <f>SUM(D46:D53)</f>
         <v>16</v>
       </c>
-      <c r="E53" s="8">
-        <f>MOD(D53,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="10"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="16" t="s">
+      <c r="E54" s="8">
+        <f>MOD(D54,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="10"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="16">
+      <c r="C56" s="16">
         <v>16</v>
       </c>
-      <c r="D55" s="16">
+      <c r="D56" s="16">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="E55" s="17" t="s">
+      <c r="E56" s="17" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C56" s="1">
-        <v>16</v>
-      </c>
-      <c r="D56" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E56" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -1684,7 +1689,7 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -1699,7 +1704,7 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -1714,7 +1719,7 @@
         <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
@@ -1729,124 +1734,124 @@
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C61" s="11">
         <v>16</v>
       </c>
-      <c r="D61" s="5">
+      <c r="D61" s="11">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="11">
+        <v>16</v>
+      </c>
+      <c r="D62" s="11">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E62" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="8" t="s">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="5">
+        <v>16</v>
+      </c>
+      <c r="D63" s="5">
+        <f t="shared" ref="D63" si="9">IF(C63="","",C63/8)</f>
+        <v>2</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C62" s="7">
-        <f>COUNT(C55:C61)</f>
-        <v>7</v>
-      </c>
-      <c r="D62" s="6">
-        <f>SUM(D55:D61)</f>
-        <v>14</v>
-      </c>
-      <c r="E62" s="8">
-        <f>MOD(D62,4)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="5"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="3"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14">
-        <v>0</v>
-      </c>
-      <c r="E64" s="15" t="s">
+      <c r="C64" s="7">
+        <f>COUNT(C56:C63)</f>
+        <v>8</v>
+      </c>
+      <c r="D64" s="6">
+        <f>SUM(D56:D63)</f>
+        <v>16</v>
+      </c>
+      <c r="E64" s="8">
+        <f>MOD(D64,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="5"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14">
+        <v>0</v>
+      </c>
+      <c r="E66" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="13"/>
-    </row>
-    <row r="66" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="7">
-        <f>D62+D64</f>
-        <v>14</v>
-      </c>
-      <c r="E66" s="8">
-        <f>MOD(D66,4)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="11"/>
-      <c r="C67" s="12"/>
+      <c r="C67" s="11"/>
       <c r="D67" s="11"/>
-      <c r="E67" s="10"/>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="16">
-        <v>8</v>
-      </c>
-      <c r="D68" s="16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E68" s="18" t="s">
+      <c r="E67" s="13"/>
+    </row>
+    <row r="68" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="7">
+        <f>D64+D66</f>
+        <v>16</v>
+      </c>
+      <c r="E68" s="8">
+        <f>MOD(D68,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="11"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="10"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="16">
+        <v>8</v>
+      </c>
+      <c r="D70" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E70" s="18" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C69" s="1">
-        <v>8</v>
-      </c>
-      <c r="D69" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" s="1">
-        <v>8</v>
-      </c>
-      <c r="D70" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
@@ -1861,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
@@ -1876,7 +1881,7 @@
         <v>1</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
@@ -1891,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
@@ -1906,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
@@ -1921,7 +1926,7 @@
         <v>1</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
@@ -1936,7 +1941,7 @@
         <v>1</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
@@ -1951,7 +1956,7 @@
         <v>1</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
@@ -1966,7 +1971,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
@@ -1981,7 +1986,7 @@
         <v>1</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
@@ -1996,7 +2001,7 @@
         <v>1</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
@@ -2011,7 +2016,7 @@
         <v>1</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
@@ -2026,7 +2031,7 @@
         <v>1</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
@@ -2041,7 +2046,7 @@
         <v>1</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
@@ -2056,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
@@ -2071,7 +2076,7 @@
         <v>1</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
@@ -2086,7 +2091,7 @@
         <v>1</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
@@ -2101,346 +2106,376 @@
         <v>1</v>
       </c>
       <c r="E87" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="1">
+        <v>8</v>
+      </c>
+      <c r="D88" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="1">
+        <v>8</v>
+      </c>
+      <c r="D89" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E89" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C88" s="11">
-        <v>8</v>
-      </c>
-      <c r="D88" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E88" s="13" t="s">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="11">
+        <v>8</v>
+      </c>
+      <c r="D90" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E90" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C89" s="11">
-        <v>8</v>
-      </c>
-      <c r="D89" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E89" s="13" t="s">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" s="11">
+        <v>8</v>
+      </c>
+      <c r="D91" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E91" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" s="1">
-        <v>8</v>
-      </c>
-      <c r="D90" s="1">
-        <f t="shared" ref="D90:D93" si="9">IF(C90="","",C90/8)</f>
-        <v>1</v>
-      </c>
-      <c r="E90" s="13" t="s">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="1">
+        <v>8</v>
+      </c>
+      <c r="D92" s="1">
+        <f t="shared" ref="D92:D95" si="10">IF(C92="","",C92/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E92" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C91" s="1">
-        <v>8</v>
-      </c>
-      <c r="D91" s="1">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E91" s="13" t="s">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1">
+        <v>8</v>
+      </c>
+      <c r="D93" s="1">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E93" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" s="11">
-        <v>8</v>
-      </c>
-      <c r="D92" s="11">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E92" s="13" t="s">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="11">
+        <v>8</v>
+      </c>
+      <c r="D94" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E94" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="11">
-        <v>8</v>
-      </c>
-      <c r="D93" s="11">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E93" s="13" t="s">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="11">
+        <v>8</v>
+      </c>
+      <c r="D95" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E95" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" s="1">
-        <v>8</v>
-      </c>
-      <c r="D94" s="1">
-        <f t="shared" ref="D94:D103" si="10">IF(C94="","",C94/8)</f>
-        <v>1</v>
-      </c>
-      <c r="E94" s="13" t="s">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="1">
+        <v>8</v>
+      </c>
+      <c r="D96" s="1">
+        <f t="shared" ref="D96:D105" si="11">IF(C96="","",C96/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E96" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C95" s="1">
-        <v>8</v>
-      </c>
-      <c r="D95" s="1">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E95" s="13" t="s">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="1">
+        <v>8</v>
+      </c>
+      <c r="D97" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E97" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" s="11">
-        <v>8</v>
-      </c>
-      <c r="D96" s="11">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E96" s="13" t="s">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="11">
+        <v>8</v>
+      </c>
+      <c r="D98" s="11">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E98" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B97" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C97" s="11">
-        <v>8</v>
-      </c>
-      <c r="D97" s="11">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E97" s="13" t="s">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" s="11">
+        <v>8</v>
+      </c>
+      <c r="D99" s="11">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E99" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B98" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="1">
-        <v>8</v>
-      </c>
-      <c r="D98" s="1">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E98" s="13" t="s">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="1">
+        <v>8</v>
+      </c>
+      <c r="D100" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E100" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B99" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C99" s="1">
-        <v>8</v>
-      </c>
-      <c r="D99" s="1">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E99" s="13" t="s">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="1">
+        <v>8</v>
+      </c>
+      <c r="D101" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E101" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="11">
-        <v>8</v>
-      </c>
-      <c r="D100" s="11">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E100" s="13" t="s">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="11">
+        <v>8</v>
+      </c>
+      <c r="D102" s="11">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E102" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B101" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C101" s="11">
-        <v>8</v>
-      </c>
-      <c r="D101" s="11">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E101" s="13" t="s">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" s="11">
+        <v>8</v>
+      </c>
+      <c r="D103" s="11">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E103" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C102" s="1">
-        <v>8</v>
-      </c>
-      <c r="D102" s="1">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E102" s="13" t="s">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1">
+        <v>8</v>
+      </c>
+      <c r="D104" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E104" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B103" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C103" s="1">
-        <v>8</v>
-      </c>
-      <c r="D103" s="1">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="E103" s="13" t="s">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="1">
+        <v>8</v>
+      </c>
+      <c r="D105" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E105" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C104" s="1">
-        <v>8</v>
-      </c>
-      <c r="D104" s="1">
-        <f>IF(C104="","",C104/8)</f>
-        <v>1</v>
-      </c>
-      <c r="E104" s="9" t="s">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="1">
+        <v>8</v>
+      </c>
+      <c r="D106" s="1">
+        <f>IF(C106="","",C106/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E106" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="8" t="s">
+    <row r="107" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C105" s="7">
-        <f>COUNT(C68:C104)</f>
+      <c r="C107" s="7">
+        <f>COUNT(C70:C106)</f>
         <v>37</v>
       </c>
-      <c r="D105" s="7">
-        <f>SUM(D68:D104)</f>
+      <c r="D107" s="7">
+        <f>SUM(D70:D106)</f>
         <v>37</v>
       </c>
-      <c r="E105" s="8">
-        <f>MOD(D105,4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="11"/>
-      <c r="C106" s="12"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="10"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B107" s="14"/>
-      <c r="C107" s="14"/>
-      <c r="D107" s="14">
-        <v>1</v>
-      </c>
-      <c r="E107" s="15" t="s">
+      <c r="E107" s="8">
+        <f>MOD(D107,4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="11"/>
+      <c r="C108" s="12"/>
+      <c r="D108" s="11"/>
+      <c r="E108" s="10"/>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B109" s="14"/>
+      <c r="C109" s="14"/>
+      <c r="D109" s="14">
+        <v>3</v>
+      </c>
+      <c r="E109" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="8"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="7">
-        <f>D105+D107</f>
-        <v>38</v>
-      </c>
-      <c r="E109" s="8">
-        <f>MOD(D109,4)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="7"/>
-      <c r="C111" s="7"/>
+    <row r="111" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B111" s="8"/>
+      <c r="C111" s="8"/>
       <c r="D111" s="7">
-        <f>SUM(D39,D43,D53,D66,D109)</f>
-        <v>224</v>
-      </c>
-      <c r="E111" s="7">
+        <f>D107+D109</f>
+        <v>40</v>
+      </c>
+      <c r="E111" s="8">
         <f>MOD(D111,4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="10"/>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="10"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="10"/>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
-      <c r="E113" s="10"/>
+    <row r="112" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="7"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="7">
+        <f>SUM(D40,D44,D54,D68,D111)</f>
+        <v>232</v>
+      </c>
+      <c r="E113" s="7">
+        <f>MOD(D113,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="10"/>
+      <c r="B114" s="11"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="10"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="10"/>
+      <c r="B115" s="11"/>
+      <c r="C115" s="11"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B64:E64">
+  <conditionalFormatting sqref="B66:E66">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$D$64&gt;0</formula>
+      <formula>$D$66&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B107:E107">
+  <conditionalFormatting sqref="B109:E109">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$D$107&gt;0</formula>
+      <formula>$D$109&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[DLG] Updated DLG.dbc and BlfConverter.py to use corrected values for DD_INA_219_shunt_voltage_raw and DD_INA_219_current_raw
</commit_message>
<xml_diff>
--- a/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
+++ b/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buderm\repositories\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandboxes\Sewela.com\smart-vibrator\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F78996-2C2A-4C98-90DF-AF83D61C62FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15904F55-6E6E-4059-86F4-4AF80C7E81C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4590" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
+    <workbookView xWindow="28680" yWindow="-3420" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -261,15 +261,9 @@
     <t>dd_ina_219_current_mA_f32</t>
   </si>
   <si>
-    <t>dd_ina_219_shunt_voltage_raw_u16</t>
-  </si>
-  <si>
     <t>dd_ina_219_power_raw_u16</t>
   </si>
   <si>
-    <t>dd_ina_219_current_raw_u16</t>
-  </si>
-  <si>
     <t>dd_ina_219_bus_voltage_raw_u16</t>
   </si>
   <si>
@@ -358,6 +352,12 @@
   </si>
   <si>
     <t>dd_tmp_102_temperature_raw_s16</t>
+  </si>
+  <si>
+    <t>dd_ina_219_shunt_voltage_raw_s16</t>
+  </si>
+  <si>
+    <t>dd_ina_219_current_raw_s16</t>
   </si>
 </sst>
 </file>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A8A1A0-79E1-4920-A494-B8E76457F73A}">
   <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,7 +870,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>41</v>
@@ -1267,7 +1267,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -1297,7 +1297,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -1311,7 +1311,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -1326,7 +1326,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
@@ -1355,7 +1355,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -1370,7 +1370,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -1385,7 +1385,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -1399,7 +1399,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -1414,7 +1414,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -1429,7 +1429,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1527,7 +1527,7 @@
         <v>16</v>
       </c>
       <c r="D46" s="16">
-        <f t="shared" ref="D46:D62" si="7">IF(C46="","",C46/8)</f>
+        <f t="shared" ref="D46:D60" si="7">IF(C46="","",C46/8)</f>
         <v>2</v>
       </c>
       <c r="E46" s="17" t="s">
@@ -1587,7 +1587,7 @@
         <v>16</v>
       </c>
       <c r="D50" s="11">
-        <f t="shared" ref="D50:D53" si="8">IF(C50="","",C50/8)</f>
+        <f t="shared" ref="D50:D51" si="8">IF(C50="","",C50/8)</f>
         <v>2</v>
       </c>
       <c r="E50" s="10" t="s">
@@ -1609,72 +1609,72 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="11">
+    <row r="52" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="7">
+        <f>COUNT(C46:C51)</f>
+        <v>6</v>
+      </c>
+      <c r="D52" s="7">
+        <f>SUM(D46:D51)</f>
+        <v>12</v>
+      </c>
+      <c r="E52" s="8">
+        <f>MOD(D52,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="16">
         <v>16</v>
       </c>
-      <c r="D52" s="11">
-        <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="11">
-        <v>16</v>
-      </c>
-      <c r="D53" s="11">
-        <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="7">
-        <f>COUNT(C46:C53)</f>
-        <v>8</v>
-      </c>
-      <c r="D54" s="7">
-        <f>SUM(D46:D53)</f>
-        <v>16</v>
-      </c>
-      <c r="E54" s="8">
-        <f>MOD(D54,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="10"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C56" s="16">
-        <v>16</v>
-      </c>
-      <c r="D56" s="16">
+      <c r="D54" s="16">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E54" s="17" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="1">
+        <v>16</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="1">
+        <v>16</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -1689,7 +1689,7 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -1704,37 +1704,37 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="11">
         <v>16</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59" s="11">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="E59" t="s">
-        <v>30</v>
+      <c r="E59" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="11">
         <v>16</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60" s="11">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="E60" t="s">
-        <v>31</v>
+      <c r="E60" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
@@ -1745,11 +1745,11 @@
         <v>16</v>
       </c>
       <c r="D61" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="D61:D62" si="9">IF(C61="","",C61/8)</f>
         <v>2</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
@@ -1760,11 +1760,11 @@
         <v>16</v>
       </c>
       <c r="D62" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
@@ -1775,11 +1775,11 @@
         <v>16</v>
       </c>
       <c r="D63" s="5">
-        <f t="shared" ref="D63" si="9">IF(C63="","",C63/8)</f>
+        <f t="shared" ref="D63" si="10">IF(C63="","",C63/8)</f>
         <v>2</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1787,12 +1787,12 @@
         <v>43</v>
       </c>
       <c r="C64" s="7">
-        <f>COUNT(C56:C63)</f>
-        <v>8</v>
+        <f>COUNT(C54:C63)</f>
+        <v>10</v>
       </c>
       <c r="D64" s="6">
-        <f>SUM(D56:D63)</f>
-        <v>16</v>
+        <f>SUM(D54:D63)</f>
+        <v>20</v>
       </c>
       <c r="E64" s="8">
         <f>MOD(D64,4)</f>
@@ -1826,7 +1826,7 @@
       <c r="C68" s="8"/>
       <c r="D68" s="7">
         <f>D64+D66</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E68" s="8">
         <f>MOD(D68,4)</f>
@@ -2177,11 +2177,11 @@
         <v>8</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" ref="D92:D95" si="10">IF(C92="","",C92/8)</f>
+        <f t="shared" ref="D92:D95" si="11">IF(C92="","",C92/8)</f>
         <v>1</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
@@ -2192,11 +2192,11 @@
         <v>8</v>
       </c>
       <c r="D93" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
@@ -2207,11 +2207,11 @@
         <v>8</v>
       </c>
       <c r="D94" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
@@ -2222,11 +2222,11 @@
         <v>8</v>
       </c>
       <c r="D95" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
@@ -2237,11 +2237,11 @@
         <v>8</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" ref="D96:D105" si="11">IF(C96="","",C96/8)</f>
+        <f t="shared" ref="D96:D105" si="12">IF(C96="","",C96/8)</f>
         <v>1</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
@@ -2252,11 +2252,11 @@
         <v>8</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
@@ -2267,11 +2267,11 @@
         <v>8</v>
       </c>
       <c r="D98" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
@@ -2282,11 +2282,11 @@
         <v>8</v>
       </c>
       <c r="D99" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
@@ -2297,11 +2297,11 @@
         <v>8</v>
       </c>
       <c r="D100" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
@@ -2312,11 +2312,11 @@
         <v>8</v>
       </c>
       <c r="D101" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
@@ -2327,11 +2327,11 @@
         <v>8</v>
       </c>
       <c r="D102" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
@@ -2342,11 +2342,11 @@
         <v>8</v>
       </c>
       <c r="D103" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
@@ -2357,11 +2357,11 @@
         <v>8</v>
       </c>
       <c r="D104" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
@@ -2372,11 +2372,11 @@
         <v>8</v>
       </c>
       <c r="D105" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
@@ -2444,7 +2444,7 @@
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7">
-        <f>SUM(D40,D44,D54,D68,D111)</f>
+        <f>SUM(D40,D44,D52,D68,D111)</f>
         <v>232</v>
       </c>
       <c r="E113" s="7">

</xml_diff>

<commit_message>
[DLG] Fixed wrong variable name dlg_time_stamp_in_sec_f32
</commit_message>
<xml_diff>
--- a/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
+++ b/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandboxes\Sewela.com\smart-vibrator\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15904F55-6E6E-4059-86F4-4AF80C7E81C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89E3726-DFB8-4861-B534-53DCFD1F8EBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3420" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
   </bookViews>
@@ -99,39 +99,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>dlg_time_stamp_f32;</t>
-  </si>
-  <si>
-    <t>icm_20600_temperature_deg_f32;</t>
-  </si>
-  <si>
-    <t>icm_20600_factory_trim_xa_f32;</t>
-  </si>
-  <si>
-    <t>icm_20600_factory_trim_ya_f32;</t>
-  </si>
-  <si>
-    <t>icm_20600_factory_trim_za_f32;</t>
-  </si>
-  <si>
-    <t>icm_20600_factory_trim_xg_f32;</t>
-  </si>
-  <si>
-    <t>icm_20600_factory_trim_yg_f32;</t>
-  </si>
-  <si>
-    <t>icm_20600_factory_trim_zg_f32;</t>
-  </si>
-  <si>
-    <t>max_30102_tenperature_f32;</t>
-  </si>
-  <si>
-    <t>max_30102_red_data_raw_u32;</t>
-  </si>
-  <si>
-    <t>max_30102_ir_data_raw_u32;</t>
-  </si>
-  <si>
     <t>icm_20600_temperature_raw_u16;</t>
   </si>
   <si>
@@ -358,13 +325,46 @@
   </si>
   <si>
     <t>dd_ina_219_current_raw_s16</t>
+  </si>
+  <si>
+    <t>dlg_time_stamp_in_sec_f32</t>
+  </si>
+  <si>
+    <t>icm_20600_temperature_deg_f32</t>
+  </si>
+  <si>
+    <t>icm_20600_factory_trim_xa_f32</t>
+  </si>
+  <si>
+    <t>icm_20600_factory_trim_ya_f32</t>
+  </si>
+  <si>
+    <t>icm_20600_factory_trim_za_f32</t>
+  </si>
+  <si>
+    <t>icm_20600_factory_trim_xg_f32</t>
+  </si>
+  <si>
+    <t>icm_20600_factory_trim_yg_f32</t>
+  </si>
+  <si>
+    <t>icm_20600_factory_trim_zg_f32</t>
+  </si>
+  <si>
+    <t>max_30102_tenperature_f32</t>
+  </si>
+  <si>
+    <t>max_30102_red_data_raw_u32</t>
+  </si>
+  <si>
+    <t>max_30102_ir_data_raw_u32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,13 +386,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -456,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -513,11 +534,77 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -855,7 +942,7 @@
   <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,23 +950,23 @@
     <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
@@ -894,7 +981,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -909,7 +996,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -924,7 +1011,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -939,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -954,7 +1041,7 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -969,7 +1056,7 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -984,7 +1071,7 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -999,7 +1086,7 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -1014,7 +1101,7 @@
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -1029,7 +1116,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -1044,7 +1131,7 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -1059,7 +1146,7 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -1074,7 +1161,7 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1089,7 +1176,7 @@
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -1104,7 +1191,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1119,7 +1206,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -1134,7 +1221,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -1149,7 +1236,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -1164,7 +1251,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -1179,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -1194,7 +1281,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1209,7 +1296,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -1224,7 +1311,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -1239,7 +1326,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -1253,7 +1340,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -1267,7 +1354,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -1282,7 +1369,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -1297,7 +1384,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -1311,7 +1398,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -1326,7 +1413,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
@@ -1341,7 +1428,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
@@ -1355,7 +1442,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -1370,7 +1457,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -1385,7 +1472,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -1399,7 +1486,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -1414,7 +1501,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -1429,7 +1516,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
@@ -1443,12 +1530,12 @@
         <v>4</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C40" s="7">
         <f>COUNT(C2:C39)</f>
@@ -1481,7 +1568,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
@@ -1496,12 +1583,12 @@
         <v>4</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C44" s="7">
         <f>COUNT(C42:C43)</f>
@@ -1531,7 +1618,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
@@ -1546,7 +1633,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
@@ -1561,7 +1648,7 @@
         <v>2</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -1576,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
@@ -1591,7 +1678,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -1606,12 +1693,12 @@
         <v>2</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C52" s="7">
         <f>COUNT(C46:C51)</f>
@@ -1644,7 +1731,7 @@
         <v>2</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -1659,7 +1746,7 @@
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -1674,7 +1761,7 @@
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -1689,7 +1776,7 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -1704,7 +1791,7 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -1719,7 +1806,7 @@
         <v>2</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
@@ -1734,7 +1821,7 @@
         <v>2</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
@@ -1749,7 +1836,7 @@
         <v>2</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
@@ -1764,7 +1851,7 @@
         <v>2</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
@@ -1779,12 +1866,12 @@
         <v>2</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C64" s="7">
         <f>COUNT(C54:C63)</f>
@@ -1812,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
@@ -1851,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
@@ -1866,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
@@ -1881,7 +1968,7 @@
         <v>1</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
@@ -1896,7 +1983,7 @@
         <v>1</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
@@ -1911,7 +1998,7 @@
         <v>1</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
@@ -1926,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
@@ -1941,7 +2028,7 @@
         <v>1</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
@@ -1956,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
@@ -1971,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
@@ -1986,7 +2073,7 @@
         <v>1</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
@@ -2151,7 +2238,7 @@
         <v>1</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
@@ -2181,7 +2268,7 @@
         <v>1</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
@@ -2196,7 +2283,7 @@
         <v>1</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
@@ -2211,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
@@ -2226,7 +2313,7 @@
         <v>1</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
@@ -2241,7 +2328,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
@@ -2256,7 +2343,7 @@
         <v>1</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
@@ -2271,7 +2358,7 @@
         <v>1</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
@@ -2286,7 +2373,7 @@
         <v>1</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
@@ -2301,7 +2388,7 @@
         <v>1</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
@@ -2316,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
@@ -2331,7 +2418,7 @@
         <v>1</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
@@ -2346,7 +2433,7 @@
         <v>1</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
@@ -2361,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
@@ -2376,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
@@ -2396,7 +2483,7 @@
     </row>
     <row r="107" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C107" s="7">
         <f>COUNT(C70:C106)</f>
@@ -2424,7 +2511,7 @@
         <v>3</v>
       </c>
       <c r="E109" s="15" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="111" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2440,19 +2527,19 @@
       </c>
     </row>
     <row r="112" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="7"/>
-      <c r="C113" s="7"/>
-      <c r="D113" s="7">
+    <row r="113" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B113" s="23"/>
+      <c r="C113" s="22"/>
+      <c r="D113" s="22">
         <f>SUM(D40,D44,D52,D68,D111)</f>
         <v>232</v>
       </c>
-      <c r="E113" s="7">
+      <c r="E113" s="22">
         <f>MOD(D113,4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
       <c r="B114" s="11"/>
       <c r="C114" s="11"/>
@@ -2469,13 +2556,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B66:E66">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$D$66&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B109:E109">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$D$109&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B113:E113">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>$E$113&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[DLG] Updated class implementation of DLG.cpp and dlg_log.cpp as well as the BlfConverter.py
</commit_message>
<xml_diff>
--- a/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
+++ b/020_Test/010_Gogeta/scripts/sbf2blf_converter/DLG_LOG_DATA.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandboxes\Sewela.com\smart-vibrator\sv-software\020_Test\010_Gogeta\scripts\sbf2blf_converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89E3726-DFB8-4861-B534-53DCFD1F8EBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190C1F8F-2090-4898-8290-4B45D048E3B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3420" windowWidth="15990" windowHeight="25440" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{55B79631-56A6-4208-A09B-8FF4C1E2A2E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$125</definedName>
+    <definedName name="dlg_types.h_1" localSheetId="0">Tabelle1!$A$2:$F$127</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="105">
   <si>
     <t>F</t>
   </si>
@@ -72,9 +72,6 @@
     <t>i2c_register_addr_u8;</t>
   </si>
   <si>
-    <t>dlg_global_msg_cnt_u8;</t>
-  </si>
-  <si>
     <t>max_30102_int_status_u8;</t>
   </si>
   <si>
@@ -358,6 +355,18 @@
   </si>
   <si>
     <t>max_30102_ir_data_raw_u32</t>
+  </si>
+  <si>
+    <t>dlg_global_msg_cnt_u8</t>
+  </si>
+  <si>
+    <t>Written with seperate fwrite() command</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -402,7 +411,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,6 +421,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -540,61 +555,31 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -939,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A8A1A0-79E1-4920-A494-B8E76457F73A}">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,246 +937,237 @@
     <col min="3" max="3" width="4.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>31</v>
-      </c>
       <c r="E1" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1">
+        <v>43</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="27">
+        <v>32</v>
+      </c>
+      <c r="D2" s="27">
         <f>IF(C2="","",C2/8)</f>
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16">
+        <v>32</v>
+      </c>
+      <c r="D4" s="16">
+        <f t="shared" ref="D4:D92" si="0">IF(C4="","",C4/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>32</v>
-      </c>
-      <c r="D3" s="1">
-        <f t="shared" ref="D3:D91" si="0">IF(C3="","",C3/8)</f>
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>32</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>32</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>32</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>32</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>32</v>
-      </c>
-      <c r="D9" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>32</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E10" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E12" t="s">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>32</v>
-      </c>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E13" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E14" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>32</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>32</v>
-      </c>
-      <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="11">
-        <v>32</v>
-      </c>
-      <c r="D16" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1206,7 +1182,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -1221,22 +1197,22 @@
         <v>4</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>32</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" ref="D19:D23" si="1">IF(C19="","",C19/8)</f>
+      <c r="B19" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="11">
+        <v>32</v>
+      </c>
+      <c r="D19" s="11">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -1247,26 +1223,26 @@
         <v>32</v>
       </c>
       <c r="D20" s="1">
+        <f t="shared" ref="D20:D24" si="1">IF(C20="","",C20/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>32</v>
+      </c>
+      <c r="D21" s="1">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="11">
-        <v>32</v>
-      </c>
-      <c r="D21" s="11">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
       <c r="E21" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -1281,7 +1257,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1296,22 +1272,22 @@
         <v>4</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
-        <v>32</v>
-      </c>
-      <c r="D24" s="1">
-        <f t="shared" ref="D24:D25" si="2">IF(C24="","",C24/8)</f>
+      <c r="B24" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="11">
+        <v>32</v>
+      </c>
+      <c r="D24" s="11">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -1322,25 +1298,26 @@
         <v>32</v>
       </c>
       <c r="D25" s="1">
+        <f t="shared" ref="D25:D26" si="2">IF(C25="","",C25/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>32</v>
+      </c>
+      <c r="D26" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="11">
-        <v>32</v>
-      </c>
-      <c r="D26" s="11">
-        <v>4</v>
-      </c>
       <c r="E26" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -1354,22 +1331,21 @@
         <v>4</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1">
-        <v>32</v>
-      </c>
-      <c r="D28" s="1">
-        <f t="shared" ref="D28:D29" si="3">IF(C28="","",C28/8)</f>
+      <c r="B28" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="11">
+        <v>32</v>
+      </c>
+      <c r="D28" s="11">
         <v>4</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -1380,40 +1356,40 @@
         <v>32</v>
       </c>
       <c r="D29" s="1">
+        <f t="shared" ref="D29:D30" si="3">IF(C29="","",C29/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>32</v>
+      </c>
+      <c r="D30" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E30" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="11">
+        <v>32</v>
+      </c>
+      <c r="D31" s="11">
+        <v>4</v>
+      </c>
+      <c r="E31" s="21" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="11">
-        <v>32</v>
-      </c>
-      <c r="D30" s="11">
-        <v>4</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
-        <v>32</v>
-      </c>
-      <c r="D31" s="1">
-        <f t="shared" ref="D31:D32" si="4">IF(C31="","",C31/8)</f>
-        <v>4</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
@@ -1424,40 +1400,40 @@
         <v>32</v>
       </c>
       <c r="D32" s="1">
+        <f t="shared" ref="D32:D33" si="4">IF(C32="","",C32/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>32</v>
+      </c>
+      <c r="D33" s="1">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E33" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="11">
+        <v>32</v>
+      </c>
+      <c r="D34" s="11">
+        <v>4</v>
+      </c>
+      <c r="E34" s="21" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="11">
-        <v>32</v>
-      </c>
-      <c r="D33" s="11">
-        <v>4</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="1">
-        <v>32</v>
-      </c>
-      <c r="D34" s="1">
-        <f t="shared" ref="D34:D35" si="5">IF(C34="","",C34/8)</f>
-        <v>4</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -1468,40 +1444,40 @@
         <v>32</v>
       </c>
       <c r="D35" s="1">
+        <f t="shared" ref="D35:D36" si="5">IF(C35="","",C35/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>32</v>
+      </c>
+      <c r="D36" s="1">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E36" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="11">
+        <v>32</v>
+      </c>
+      <c r="D37" s="11">
+        <v>4</v>
+      </c>
+      <c r="E37" s="21" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="11">
-        <v>32</v>
-      </c>
-      <c r="D36" s="11">
-        <v>4</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="1">
-        <v>32</v>
-      </c>
-      <c r="D37" s="1">
-        <f t="shared" ref="D37:D38" si="6">IF(C37="","",C37/8)</f>
-        <v>4</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -1512,128 +1488,128 @@
         <v>32</v>
       </c>
       <c r="D38" s="1">
+        <f t="shared" ref="D38:D39" si="6">IF(C38="","",C38/8)</f>
+        <v>4</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1">
+        <v>32</v>
+      </c>
+      <c r="D39" s="1">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="E38" s="21" t="s">
+      <c r="E39" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="11">
+        <v>32</v>
+      </c>
+      <c r="D40" s="11">
+        <v>4</v>
+      </c>
+      <c r="E40" s="21" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="11">
-        <v>32</v>
-      </c>
-      <c r="D39" s="11">
-        <v>4</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="7">
-        <f>COUNT(C2:C39)</f>
-        <v>38</v>
-      </c>
-      <c r="D40" s="7">
-        <f>SUM(D2:D39)</f>
-        <v>152</v>
-      </c>
-      <c r="E40" s="8">
-        <f>MOD(D40,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D41" s="1" t="str">
+    <row r="41" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="7">
+        <f>COUNT(C4:C40)</f>
+        <v>37</v>
+      </c>
+      <c r="D41" s="7">
+        <f>SUM(D4:D40)</f>
+        <v>148</v>
+      </c>
+      <c r="E41" s="8">
+        <f>MOD(D41,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="16">
-        <v>32</v>
-      </c>
-      <c r="D42" s="16">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E42" s="17" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="16">
+        <v>32</v>
+      </c>
+      <c r="D43" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="5">
+        <v>32</v>
+      </c>
+      <c r="D44" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="5">
-        <v>32</v>
-      </c>
-      <c r="D43" s="5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="7">
-        <f>COUNT(C42:C43)</f>
+    <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="7">
+        <f>COUNT(C43:C44)</f>
         <v>2</v>
       </c>
-      <c r="D44" s="7">
-        <f>SUM(D42:D43)</f>
-        <v>8</v>
-      </c>
-      <c r="E44" s="8">
-        <f>MOD(D44,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="2"/>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="16">
+      <c r="D45" s="7">
+        <f>SUM(D43:D44)</f>
+        <v>8</v>
+      </c>
+      <c r="E45" s="8">
+        <f>MOD(D45,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="16">
         <v>16</v>
       </c>
-      <c r="D46" s="16">
-        <f t="shared" ref="D46:D60" si="7">IF(C46="","",C46/8)</f>
+      <c r="D47" s="16">
+        <f t="shared" ref="D47:D61" si="7">IF(C47="","",C47/8)</f>
         <v>2</v>
       </c>
-      <c r="E46" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="11">
-        <v>16</v>
-      </c>
-      <c r="D47" s="11">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>47</v>
+      <c r="E47" s="17" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
@@ -1648,7 +1624,7 @@
         <v>2</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -1663,7 +1639,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
@@ -1674,11 +1650,11 @@
         <v>16</v>
       </c>
       <c r="D50" s="11">
-        <f t="shared" ref="D50:D51" si="8">IF(C50="","",C50/8)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -1689,69 +1665,69 @@
         <v>16</v>
       </c>
       <c r="D51" s="11">
+        <f t="shared" ref="D51:D52" si="8">IF(C51="","",C51/8)</f>
+        <v>2</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="11">
+        <v>16</v>
+      </c>
+      <c r="D52" s="11">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="E51" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" s="7">
-        <f>COUNT(C46:C51)</f>
+      <c r="E52" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="7">
+        <f>COUNT(C47:C52)</f>
         <v>6</v>
       </c>
-      <c r="D52" s="7">
-        <f>SUM(D46:D51)</f>
+      <c r="D53" s="7">
+        <f>SUM(D47:D52)</f>
         <v>12</v>
       </c>
-      <c r="E52" s="8">
-        <f>MOD(D52,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="10"/>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="16">
+      <c r="E53" s="8">
+        <f>MOD(D53,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="16">
         <v>16</v>
       </c>
-      <c r="D54" s="16">
+      <c r="D55" s="16">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="E54" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55" s="1">
-        <v>16</v>
-      </c>
-      <c r="D55" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E55" t="s">
-        <v>17</v>
+      <c r="E55" s="17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C56" s="1">
         <v>16</v>
@@ -1761,12 +1737,12 @@
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C57" s="1">
         <v>16</v>
@@ -1776,12 +1752,12 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C58" s="1">
         <v>16</v>
@@ -1791,27 +1767,27 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" s="11">
+      <c r="B59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="1">
         <v>16</v>
       </c>
-      <c r="D59" s="11">
+      <c r="D59" s="1">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="E59" s="10" t="s">
-        <v>21</v>
+      <c r="E59" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C60" s="11">
         <v>16</v>
@@ -1821,139 +1797,139 @@
         <v>2</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C61" s="11">
         <v>16</v>
       </c>
       <c r="D61" s="11">
-        <f t="shared" ref="D61:D62" si="9">IF(C61="","",C61/8)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C62" s="11">
         <v>16</v>
       </c>
       <c r="D62" s="11">
+        <f t="shared" ref="D62:D63" si="9">IF(C62="","",C62/8)</f>
+        <v>2</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="11">
+        <v>16</v>
+      </c>
+      <c r="D63" s="11">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="E62" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C63" s="5">
+      <c r="E63" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="5">
         <v>16</v>
       </c>
-      <c r="D63" s="5">
-        <f t="shared" ref="D63" si="10">IF(C63="","",C63/8)</f>
+      <c r="D64" s="5">
+        <f t="shared" ref="D64" si="10">IF(C64="","",C64/8)</f>
         <v>2</v>
       </c>
-      <c r="E63" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C64" s="7">
-        <f>COUNT(C54:C63)</f>
+      <c r="E64" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" s="7">
+        <f>COUNT(C55:C64)</f>
         <v>10</v>
       </c>
-      <c r="D64" s="6">
-        <f>SUM(D54:D63)</f>
+      <c r="D65" s="6">
+        <f>SUM(D55:D64)</f>
         <v>20</v>
       </c>
-      <c r="E64" s="8">
-        <f>MOD(D64,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="5"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14">
-        <v>0</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="E65" s="8">
+        <f>MOD(D65,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="5"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="3"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="13"/>
-    </row>
-    <row r="68" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="7">
-        <f>D64+D66</f>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14">
+        <v>0</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="13"/>
+    </row>
+    <row r="69" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="7">
+        <f>D65+D67</f>
         <v>20</v>
       </c>
-      <c r="E68" s="8">
-        <f>MOD(D68,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="11"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="10"/>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" s="16">
-        <v>8</v>
-      </c>
-      <c r="D70" s="16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E70" s="18" t="s">
-        <v>33</v>
-      </c>
+      <c r="E69" s="8">
+        <f>MOD(D69,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="11"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="10"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="1">
-        <v>8</v>
-      </c>
-      <c r="D71" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>35</v>
+      <c r="B71" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="16">
+        <v>8</v>
+      </c>
+      <c r="D71" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E71" s="18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
@@ -1968,7 +1944,7 @@
         <v>1</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
@@ -1983,7 +1959,7 @@
         <v>1</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
@@ -1998,7 +1974,7 @@
         <v>1</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
@@ -2013,7 +1989,7 @@
         <v>1</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
@@ -2028,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
@@ -2043,7 +2019,7 @@
         <v>1</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
@@ -2058,7 +2034,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
@@ -2073,7 +2049,7 @@
         <v>1</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
@@ -2088,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
@@ -2103,7 +2079,7 @@
         <v>1</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
@@ -2118,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
@@ -2133,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
@@ -2148,7 +2124,7 @@
         <v>1</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
@@ -2163,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
@@ -2178,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
@@ -2193,7 +2169,7 @@
         <v>1</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
@@ -2208,7 +2184,7 @@
         <v>1</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
@@ -2223,22 +2199,22 @@
         <v>1</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" s="11">
-        <v>8</v>
-      </c>
-      <c r="D90" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E90" s="13" t="s">
-        <v>29</v>
+      <c r="B90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="1">
+        <v>8</v>
+      </c>
+      <c r="D90" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
@@ -2253,22 +2229,22 @@
         <v>1</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" s="1">
-        <v>8</v>
-      </c>
-      <c r="D92" s="1">
-        <f t="shared" ref="D92:D95" si="11">IF(C92="","",C92/8)</f>
+      <c r="B92" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="11">
+        <v>8</v>
+      </c>
+      <c r="D92" s="11">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
@@ -2279,26 +2255,26 @@
         <v>8</v>
       </c>
       <c r="D93" s="1">
+        <f t="shared" ref="D93:D96" si="11">IF(C93="","",C93/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E93" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="1">
+        <v>8</v>
+      </c>
+      <c r="D94" s="1">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="E93" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" s="11">
-        <v>8</v>
-      </c>
-      <c r="D94" s="11">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
       <c r="E94" s="13" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
@@ -2313,55 +2289,55 @@
         <v>1</v>
       </c>
       <c r="E95" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="11">
+        <v>8</v>
+      </c>
+      <c r="D96" s="11">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="1">
+        <v>8</v>
+      </c>
+      <c r="D97" s="1">
+        <f t="shared" ref="D97:D106" si="12">IF(C97="","",C97/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E97" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" s="1">
-        <v>8</v>
-      </c>
-      <c r="D96" s="1">
-        <f t="shared" ref="D96:D105" si="12">IF(C96="","",C96/8)</f>
-        <v>1</v>
-      </c>
-      <c r="E96" s="13" t="s">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="1">
+        <v>8</v>
+      </c>
+      <c r="D98" s="1">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E98" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B97" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C97" s="1">
-        <v>8</v>
-      </c>
-      <c r="D97" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E97" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B98" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="11">
-        <v>8</v>
-      </c>
-      <c r="D98" s="11">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E98" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="11" t="s">
         <v>1</v>
       </c>
@@ -2373,25 +2349,25 @@
         <v>1</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="1">
-        <v>8</v>
-      </c>
-      <c r="D100" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B100" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="11">
+        <v>8</v>
+      </c>
+      <c r="D100" s="11">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
         <v>1</v>
       </c>
@@ -2403,25 +2379,25 @@
         <v>1</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C102" s="11">
-        <v>8</v>
-      </c>
-      <c r="D102" s="11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="1">
+        <v>8</v>
+      </c>
+      <c r="D102" s="1">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="11" t="s">
         <v>1</v>
       </c>
@@ -2433,25 +2409,25 @@
         <v>1</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C104" s="1">
-        <v>8</v>
-      </c>
-      <c r="D104" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B104" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="11">
+        <v>8</v>
+      </c>
+      <c r="D104" s="11">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
         <v>1</v>
       </c>
@@ -2463,111 +2439,143 @@
         <v>1</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B106" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C106" s="1">
-        <v>8</v>
-      </c>
-      <c r="D106" s="1">
-        <f>IF(C106="","",C106/8)</f>
-        <v>1</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B106" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="5">
+        <v>8</v>
+      </c>
+      <c r="D106" s="5">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E106" s="24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C107" s="7">
-        <f>COUNT(C70:C106)</f>
-        <v>37</v>
+        <f>COUNT(C71:C106)</f>
+        <v>36</v>
       </c>
       <c r="D107" s="7">
-        <f>SUM(D70:D106)</f>
-        <v>37</v>
+        <f>SUM(D71:D106)</f>
+        <v>36</v>
       </c>
       <c r="E107" s="8">
         <f>MOD(D107,4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B108" s="11"/>
       <c r="C108" s="12"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="10"/>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B109" s="14"/>
-      <c r="C109" s="14"/>
-      <c r="D109" s="14">
-        <v>3</v>
-      </c>
-      <c r="E109" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="111" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="8"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="7">
-        <f>D107+D109</f>
-        <v>40</v>
-      </c>
-      <c r="E111" s="8">
-        <f>MOD(D111,4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B113" s="23"/>
-      <c r="C113" s="22"/>
-      <c r="D113" s="22">
-        <f>SUM(D40,D44,D52,D68,D111)</f>
-        <v>232</v>
-      </c>
-      <c r="E113" s="22">
+      <c r="D108" s="12"/>
+      <c r="E108" s="11"/>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B109" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="25">
+        <v>8</v>
+      </c>
+      <c r="D109" s="25">
+        <f>IF(C109="","",C109/8)</f>
+        <v>1</v>
+      </c>
+      <c r="E109" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B110" s="11"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="10"/>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B111" s="14"/>
+      <c r="C111" s="14"/>
+      <c r="D111" s="14">
+        <v>0</v>
+      </c>
+      <c r="E111" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="7">
+        <f>D107+D111</f>
+        <v>36</v>
+      </c>
+      <c r="E113" s="8">
         <f>MOD(D113,4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="10"/>
-      <c r="B114" s="11"/>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="10"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="10"/>
-      <c r="B115" s="11"/>
-      <c r="C115" s="11"/>
-      <c r="D115" s="11"/>
-      <c r="E115" s="10"/>
+    <row r="114" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B115" s="23"/>
+      <c r="C115" s="22"/>
+      <c r="D115" s="22">
+        <f>SUM(D41,D45,D53,D69,D113)</f>
+        <v>224</v>
+      </c>
+      <c r="E115" s="22">
+        <f>MOD(D115,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="10"/>
+      <c r="B116" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C116" s="31"/>
+      <c r="D116" s="7">
+        <f>SUM(D2,D109,D115)</f>
+        <v>229</v>
+      </c>
+      <c r="E116" s="30"/>
+    </row>
+    <row r="117" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="10"/>
+      <c r="B117" s="11"/>
+      <c r="C117" s="11"/>
+      <c r="D117" s="11"/>
+      <c r="E117" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B116:C116"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B66:E66">
-    <cfRule type="expression" dxfId="7" priority="3">
-      <formula>$D$66&gt;0</formula>
+  <conditionalFormatting sqref="B67:E67">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$D$67&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B109:E109">
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>$D$109&gt;0</formula>
+  <conditionalFormatting sqref="B111:E111">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$D$111&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B113:E113">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>$E$113&lt;&gt;0</formula>
+  <conditionalFormatting sqref="B115:E115">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$E$115&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>